<commit_message>
color rojo y condicion dias seguidos
</commit_message>
<xml_diff>
--- a/Cronograma-2026-01-01-2026-01-15.xlsx
+++ b/Cronograma-2026-01-01-2026-01-15.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="71">
   <si>
     <t>Puestos</t>
   </si>
@@ -323,7 +323,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -646,9 +653,12 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -733,16 +743,16 @@
         <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N2" t="s">
         <v>60</v>
@@ -751,7 +761,7 @@
         <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="Q2" t="s">
         <v>60</v>
@@ -783,31 +793,31 @@
         <v>66</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
         <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="O3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -842,22 +852,22 @@
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="M4" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="P4" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
         <v>33</v>
@@ -889,31 +899,31 @@
         <v>53</v>
       </c>
       <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" t="s">
-        <v>54</v>
-      </c>
       <c r="Q5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -941,32 +951,29 @@
       <c r="H6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>50</v>
-      </c>
       <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
         <v>36</v>
       </c>
-      <c r="L6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" t="s">
-        <v>56</v>
-      </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -994,32 +1001,23 @@
       <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
       <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" t="s">
         <v>50</v>
       </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="N7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7" t="s">
-        <v>62</v>
-      </c>
-      <c r="P7" t="s">
-        <v>56</v>
-      </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1047,32 +1045,20 @@
       <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" t="s">
-        <v>37</v>
-      </c>
       <c r="K8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L8" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="N8" t="s">
         <v>66</v>
       </c>
       <c r="O8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1160,13 +1146,13 @@
         <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
         <v>39</v>
@@ -1175,7 +1161,7 @@
         <v>39</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="Q10" t="s">
         <v>39</v>
@@ -1206,11 +1192,8 @@
       <c r="H11" t="s">
         <v>46</v>
       </c>
-      <c r="I11" t="s">
-        <v>57</v>
-      </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
         <v>41</v>
@@ -1219,19 +1202,16 @@
         <v>41</v>
       </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="O11" t="s">
         <v>57</v>
       </c>
-      <c r="P11" t="s">
-        <v>40</v>
-      </c>
       <c r="Q11" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1256,35 +1236,26 @@
       <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="s">
         <v>40</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>46</v>
       </c>
-      <c r="J12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
       <c r="M12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" t="s">
         <v>41</v>
       </c>
-      <c r="N12" t="s">
-        <v>40</v>
-      </c>
       <c r="O12" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" t="s">
         <v>46</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1312,11 +1283,8 @@
       <c r="H13" t="s">
         <v>59</v>
       </c>
-      <c r="I13" t="s">
-        <v>59</v>
-      </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="K13" t="s">
         <v>59</v>
@@ -1325,19 +1293,16 @@
         <v>59</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P13" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1365,31 +1330,19 @@
       <c r="H14" t="s">
         <v>65</v>
       </c>
-      <c r="I14" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" t="s">
-        <v>65</v>
-      </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="N14" t="s">
         <v>43</v>
       </c>
       <c r="O14" t="s">
-        <v>43</v>
-      </c>
-      <c r="P14" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1425,13 +1378,13 @@
         <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L15" t="s">
         <v>44</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N15" t="s">
         <v>44</v>
@@ -1443,7 +1396,7 @@
         <v>44</v>
       </c>
       <c r="Q15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1471,32 +1424,20 @@
       <c r="H16" t="s">
         <v>58</v>
       </c>
-      <c r="I16" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" t="s">
-        <v>58</v>
-      </c>
       <c r="K16" t="s">
         <v>58</v>
       </c>
       <c r="L16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="N16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="O16" t="s">
-        <v>45</v>
-      </c>
-      <c r="P16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1521,15 +1462,6 @@
       <c r="G17" t="s">
         <v>34</v>
       </c>
-      <c r="H17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" t="s">
-        <v>46</v>
-      </c>
       <c r="K17" t="s">
         <v>34</v>
       </c>
@@ -1540,15 +1472,9 @@
         <v>34</v>
       </c>
       <c r="N17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="O17" t="s">
-        <v>46</v>
-      </c>
-      <c r="P17" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q17" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1574,17 +1500,8 @@
       <c r="G18" t="s">
         <v>47</v>
       </c>
-      <c r="H18" t="s">
+      <c r="K18" t="s">
         <v>47</v>
-      </c>
-      <c r="I18" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" t="s">
-        <v>46</v>
       </c>
       <c r="L18" t="s">
         <v>47</v>
@@ -1596,12 +1513,6 @@
         <v>47</v>
       </c>
       <c r="O18" t="s">
-        <v>47</v>
-      </c>
-      <c r="P18" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1627,12 +1538,6 @@
       <c r="G19" t="s">
         <v>48</v>
       </c>
-      <c r="H19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" t="s">
-        <v>48</v>
-      </c>
       <c r="J19" t="s">
         <v>48</v>
       </c>
@@ -1646,12 +1551,6 @@
         <v>48</v>
       </c>
       <c r="N19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O19" t="s">
-        <v>48</v>
-      </c>
-      <c r="P19" t="s">
         <v>48</v>
       </c>
       <c r="Q19" t="s">
@@ -1680,12 +1579,6 @@
       <c r="G20" t="s">
         <v>49</v>
       </c>
-      <c r="H20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" t="s">
-        <v>49</v>
-      </c>
       <c r="J20" t="s">
         <v>49</v>
       </c>
@@ -1699,12 +1592,6 @@
         <v>49</v>
       </c>
       <c r="N20" t="s">
-        <v>49</v>
-      </c>
-      <c r="O20" t="s">
-        <v>49</v>
-      </c>
-      <c r="P20" t="s">
         <v>49</v>
       </c>
       <c r="Q20" t="s">
@@ -1736,32 +1623,23 @@
       <c r="H21" t="s">
         <v>55</v>
       </c>
-      <c r="I21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" t="s">
-        <v>54</v>
-      </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="L21" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="M21" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="N21" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="O21" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="P21" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1789,32 +1667,23 @@
       <c r="H22" t="s">
         <v>56</v>
       </c>
-      <c r="I22" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" t="s">
-        <v>31</v>
-      </c>
       <c r="K22" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="L22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="N22" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="O22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P22" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1842,32 +1711,20 @@
       <c r="H23" t="s">
         <v>61</v>
       </c>
-      <c r="I23" t="s">
+      <c r="L23" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" t="s">
         <v>52</v>
       </c>
-      <c r="J23" t="s">
-        <v>52</v>
-      </c>
-      <c r="K23" t="s">
-        <v>62</v>
-      </c>
-      <c r="L23" t="s">
-        <v>55</v>
-      </c>
-      <c r="M23" t="s">
-        <v>54</v>
-      </c>
       <c r="N23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O23" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="P23" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1895,32 +1752,20 @@
       <c r="H24" t="s">
         <v>62</v>
       </c>
-      <c r="I24" t="s">
+      <c r="L24" t="s">
         <v>55</v>
       </c>
-      <c r="J24" t="s">
+      <c r="M24" t="s">
+        <v>54</v>
+      </c>
+      <c r="N24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" t="s">
         <v>53</v>
       </c>
-      <c r="K24" t="s">
-        <v>63</v>
-      </c>
-      <c r="L24" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O24" t="s">
-        <v>35</v>
-      </c>
       <c r="P24" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1948,32 +1793,17 @@
       <c r="H25" t="s">
         <v>63</v>
       </c>
-      <c r="I25" t="s">
+      <c r="L25" t="s">
         <v>56</v>
       </c>
-      <c r="J25" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" t="s">
+        <v>52</v>
+      </c>
+      <c r="O25" t="s">
         <v>31</v>
-      </c>
-      <c r="L25" t="s">
-        <v>61</v>
-      </c>
-      <c r="M25" t="s">
-        <v>53</v>
-      </c>
-      <c r="N25" t="s">
-        <v>53</v>
-      </c>
-      <c r="O25" t="s">
-        <v>36</v>
-      </c>
-      <c r="P25" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1998,35 +1828,17 @@
       <c r="G26" t="s">
         <v>36</v>
       </c>
-      <c r="H26" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="L26" t="s">
         <v>61</v>
       </c>
-      <c r="J26" t="s">
-        <v>55</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" t="s">
         <v>35</v>
-      </c>
-      <c r="L26" t="s">
-        <v>62</v>
-      </c>
-      <c r="M26" t="s">
-        <v>55</v>
-      </c>
-      <c r="N26" t="s">
-        <v>51</v>
-      </c>
-      <c r="O26" t="s">
-        <v>53</v>
-      </c>
-      <c r="P26" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2051,35 +1863,17 @@
       <c r="G27" t="s">
         <v>37</v>
       </c>
-      <c r="H27" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="L27" t="s">
         <v>51</v>
       </c>
-      <c r="J27" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" t="s">
-        <v>63</v>
-      </c>
       <c r="M27" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="O27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P27" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2104,35 +1898,14 @@
       <c r="G28" t="s">
         <v>41</v>
       </c>
-      <c r="H28" t="s">
-        <v>41</v>
-      </c>
-      <c r="I28" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" t="s">
-        <v>40</v>
-      </c>
       <c r="L28" t="s">
         <v>40</v>
       </c>
       <c r="M28" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="N28" t="s">
-        <v>41</v>
-      </c>
-      <c r="O28" t="s">
-        <v>41</v>
-      </c>
-      <c r="P28" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2157,35 +1930,20 @@
       <c r="G29" t="s">
         <v>45</v>
       </c>
-      <c r="H29" t="s">
+      <c r="K29" t="s">
         <v>45</v>
       </c>
-      <c r="I29" t="s">
+      <c r="L29" t="s">
         <v>45</v>
       </c>
-      <c r="J29" t="s">
+      <c r="M29" t="s">
         <v>45</v>
       </c>
-      <c r="K29" t="s">
-        <v>66</v>
-      </c>
-      <c r="L29" t="s">
-        <v>58</v>
-      </c>
-      <c r="M29" t="s">
-        <v>58</v>
-      </c>
       <c r="N29" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="O29" t="s">
-        <v>58</v>
-      </c>
-      <c r="P29" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2210,20 +1968,11 @@
       <c r="G30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" t="s">
-        <v>43</v>
-      </c>
-      <c r="J30" t="s">
-        <v>43</v>
-      </c>
       <c r="K30" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="L30" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="M30" t="s">
         <v>65</v>
@@ -2234,14 +1983,13 @@
       <c r="O30" t="s">
         <v>65</v>
       </c>
-      <c r="P30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:Q30">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C2=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5095,30 +4843,30 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <conditionalFormatting sqref="B2:B37">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D37">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:S37">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>VLOOKUP((E2),Cronograma!$A$2:$B$30,2,FALSE)=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>VLOOKUP((E2),Cronograma!$A$2:$B$30,2,FALSE)=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:S37">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(NOT(IFERROR(VLOOKUP((E2),Cronograma!$A$2:$B$30,2,FALSE), FALSE)=TRUE), F2="")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Grafo con pesos constantes
</commit_message>
<xml_diff>
--- a/Cronograma-2026-01-01-2026-01-15.xlsx
+++ b/Cronograma-2026-01-01-2026-01-15.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="71">
   <si>
     <t>Puestos</t>
   </si>
@@ -132,112 +132,112 @@
     <t>N - Barra y salón</t>
   </si>
   <si>
+    <t>Betsy Mauribel</t>
+  </si>
+  <si>
+    <t>Gilvert</t>
+  </si>
+  <si>
+    <t>Efigenia</t>
+  </si>
+  <si>
+    <t>Dora</t>
+  </si>
+  <si>
+    <t>German Avila</t>
+  </si>
+  <si>
+    <t>Angie Castillo</t>
+  </si>
+  <si>
+    <t>Erika Mayerlli</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Adriana</t>
+  </si>
+  <si>
+    <t>Claudia Patricia</t>
+  </si>
+  <si>
+    <t>Ofelia</t>
+  </si>
+  <si>
+    <t>Maria Alejandra</t>
+  </si>
+  <si>
+    <t>Maria Naydu</t>
+  </si>
+  <si>
+    <t>Tatiana</t>
+  </si>
+  <si>
+    <t>Rosalba</t>
+  </si>
+  <si>
+    <t>Luz Mery</t>
+  </si>
+  <si>
+    <t>Jeferson</t>
+  </si>
+  <si>
+    <t>Claudia Milena</t>
+  </si>
+  <si>
+    <t>Victor Julio</t>
+  </si>
+  <si>
+    <t>Yenifer</t>
+  </si>
+  <si>
+    <t>Xiomara</t>
+  </si>
+  <si>
+    <t>Rosa Angelica</t>
+  </si>
+  <si>
+    <t>Darcy Lorena</t>
+  </si>
+  <si>
+    <t>Maribel</t>
+  </si>
+  <si>
+    <t>Maria Paula</t>
+  </si>
+  <si>
+    <t>Luisa Viviana</t>
+  </si>
+  <si>
+    <t>Luz Estela</t>
+  </si>
+  <si>
+    <t>Angie Marcela</t>
+  </si>
+  <si>
+    <t>Carolina</t>
+  </si>
+  <si>
+    <t>Stefany</t>
+  </si>
+  <si>
+    <t>Diana Carolina Molina</t>
+  </si>
+  <si>
+    <t>Elisa Parra</t>
+  </si>
+  <si>
+    <t>Anyelis</t>
+  </si>
+  <si>
+    <t>Alba Becerra</t>
+  </si>
+  <si>
     <t>Adanies</t>
   </si>
   <si>
-    <t>Alba Becerra</t>
-  </si>
-  <si>
-    <t>Efigenia</t>
-  </si>
-  <si>
-    <t>Angie Castillo</t>
-  </si>
-  <si>
-    <t>Anyelis</t>
-  </si>
-  <si>
-    <t>Darcy Lorena</t>
-  </si>
-  <si>
-    <t>Elisa Parra</t>
-  </si>
-  <si>
     <t>Gisela</t>
-  </si>
-  <si>
-    <t>Adriana</t>
-  </si>
-  <si>
-    <t>Claudia Patricia</t>
-  </si>
-  <si>
-    <t>Luz Estela</t>
-  </si>
-  <si>
-    <t>Dora</t>
-  </si>
-  <si>
-    <t>Carolina</t>
-  </si>
-  <si>
-    <t>Tatiana</t>
-  </si>
-  <si>
-    <t>Angie Marcela</t>
-  </si>
-  <si>
-    <t>Luz Mery</t>
-  </si>
-  <si>
-    <t>Jeferson</t>
-  </si>
-  <si>
-    <t>Claudia Milena</t>
-  </si>
-  <si>
-    <t>Victor Julio</t>
-  </si>
-  <si>
-    <t>Luisa Viviana</t>
-  </si>
-  <si>
-    <t>Maria Paula</t>
-  </si>
-  <si>
-    <t>Maribel</t>
-  </si>
-  <si>
-    <t>German Avila</t>
-  </si>
-  <si>
-    <t>Rosa Angelica</t>
-  </si>
-  <si>
-    <t>Xiomara</t>
-  </si>
-  <si>
-    <t>Yenifer</t>
-  </si>
-  <si>
-    <t>Ofelia</t>
-  </si>
-  <si>
-    <t>Rosalba</t>
-  </si>
-  <si>
-    <t>Maria Naydu</t>
-  </si>
-  <si>
-    <t>Diana Carolina Molina</t>
-  </si>
-  <si>
-    <t>Erika Mayerlli</t>
-  </si>
-  <si>
-    <t>Gilvert</t>
-  </si>
-  <si>
-    <t>Betsy Mauribel</t>
-  </si>
-  <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Maria Alejandra</t>
-  </si>
-  <si>
-    <t>Stefany</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -650,15 +650,10 @@
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -725,46 +720,46 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -778,22 +773,22 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
         <v>32</v>
@@ -808,16 +803,16 @@
         <v>50</v>
       </c>
       <c r="N3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" t="s">
         <v>56</v>
-      </c>
-      <c r="P3" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -831,10 +826,10 @@
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
         <v>33</v>
@@ -843,31 +838,31 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Q4" t="s">
         <v>33</v>
@@ -884,46 +879,46 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
         <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="P5" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -937,43 +932,46 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
         <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -987,37 +985,46 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" t="s">
         <v>63</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
+      <c r="P7" t="s">
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1031,34 +1038,37 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1072,43 +1082,43 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
         <v>38</v>
-      </c>
-      <c r="J9" t="s">
-        <v>64</v>
       </c>
       <c r="K9" t="s">
         <v>38</v>
       </c>
       <c r="L9" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="M9" t="s">
         <v>38</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="O9" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q9" t="s">
         <v>38</v>
@@ -1128,40 +1138,31 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
         <v>39</v>
       </c>
       <c r="J10" t="s">
         <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="N10" t="s">
         <v>39</v>
       </c>
       <c r="O10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="Q10" t="s">
         <v>39</v>
@@ -1184,30 +1185,24 @@
         <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="M11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="N11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" t="s">
         <v>57</v>
       </c>
       <c r="Q11" t="s">
@@ -1231,31 +1226,28 @@
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N12" t="s">
         <v>41</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>41</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1269,37 +1261,34 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K13" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="M13" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="N13" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="O13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
         <v>42</v>
@@ -1322,13 +1311,13 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
+        <v>43</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
       </c>
       <c r="K14" t="s">
         <v>43</v>
@@ -1342,7 +1331,7 @@
       <c r="N14" t="s">
         <v>43</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1357,7 +1346,7 @@
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
         <v>44</v>
@@ -1366,33 +1355,21 @@
         <v>44</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" t="s">
         <v>44</v>
       </c>
       <c r="J15" t="s">
         <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L15" t="s">
         <v>44</v>
       </c>
       <c r="M15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15" t="s">
         <v>44</v>
       </c>
       <c r="Q15" t="s">
@@ -1416,28 +1393,28 @@
         <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="J16" t="s">
+        <v>45</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="L16" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="N16" t="s">
-        <v>58</v>
-      </c>
-      <c r="O16" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1451,31 +1428,34 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="L17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="N17" t="s">
         <v>46</v>
       </c>
-      <c r="O17" t="s">
-        <v>34</v>
+      <c r="Q17" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1512,9 +1492,6 @@
       <c r="N18" t="s">
         <v>47</v>
       </c>
-      <c r="O18" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
@@ -1609,19 +1586,22 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="J21" t="s">
+        <v>56</v>
       </c>
       <c r="K21" t="s">
         <v>31</v>
@@ -1633,13 +1613,16 @@
         <v>31</v>
       </c>
       <c r="N21" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="O21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="P21" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1653,37 +1636,40 @@
         <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" t="s">
         <v>37</v>
       </c>
-      <c r="F22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" t="s">
-        <v>56</v>
-      </c>
-      <c r="K22" t="s">
-        <v>54</v>
-      </c>
       <c r="L22" t="s">
+        <v>37</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22" t="s">
         <v>52</v>
       </c>
-      <c r="M22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" t="s">
-        <v>63</v>
-      </c>
-      <c r="O22" t="s">
-        <v>62</v>
-      </c>
       <c r="P22" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1697,34 +1683,40 @@
         <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" t="s">
+        <v>56</v>
       </c>
       <c r="L23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
         <v>54</v>
       </c>
-      <c r="M23" t="s">
-        <v>52</v>
-      </c>
-      <c r="N23" t="s">
-        <v>31</v>
-      </c>
-      <c r="O23" t="s">
-        <v>63</v>
-      </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1738,34 +1730,40 @@
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
         <v>63</v>
       </c>
-      <c r="H24" t="s">
+      <c r="K24" t="s">
         <v>62</v>
       </c>
       <c r="L24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N24" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="O24" t="s">
         <v>53</v>
       </c>
       <c r="P24" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1779,31 +1777,37 @@
         <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
         <v>63</v>
       </c>
       <c r="L25" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="M25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N25" t="s">
         <v>52</v>
       </c>
       <c r="O25" t="s">
-        <v>31</v>
+        <v>55</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1817,28 +1821,34 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="J26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" t="s">
+        <v>53</v>
       </c>
       <c r="L26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N26" t="s">
         <v>54</v>
       </c>
-      <c r="O26" t="s">
-        <v>35</v>
+      <c r="Q26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1852,28 +1862,31 @@
         <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>55</v>
+      </c>
+      <c r="K27" t="s">
+        <v>65</v>
       </c>
       <c r="L27" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="M27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="N27" t="s">
         <v>55</v>
       </c>
-      <c r="O27" t="s">
-        <v>52</v>
+      <c r="Q27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1893,10 +1906,16 @@
         <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>57</v>
+      </c>
+      <c r="J28" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" t="s">
+        <v>40</v>
       </c>
       <c r="L28" t="s">
         <v>40</v>
@@ -1925,25 +1944,28 @@
         <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="L29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="M29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="N29" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="O29" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1963,25 +1985,25 @@
         <v>59</v>
       </c>
       <c r="F30" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="K30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="N30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O30" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2070,7 +2092,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E2:S2, Cronograma!A2:A30)))</f>
@@ -2147,7 +2169,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E3:S3, Cronograma!A2:A30)))</f>
@@ -2224,7 +2246,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E4:S4, Cronograma!A2:A30)))</f>
@@ -2301,7 +2323,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E5:S5, Cronograma!A2:A30)))</f>
@@ -2378,7 +2400,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E6:S6, Cronograma!A2:A30)))</f>
@@ -2455,7 +2477,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E7:S7, Cronograma!A2:A30)))</f>
@@ -2609,7 +2631,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E9:S9, Cronograma!A2:A30)))</f>
@@ -2686,7 +2708,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E10:S10, Cronograma!A2:A30)))</f>
@@ -2763,7 +2785,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B11">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E11:S11, Cronograma!A2:A30)))</f>
@@ -2840,7 +2862,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E12:S12, Cronograma!A2:A30)))</f>
@@ -2917,7 +2939,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E13:S13, Cronograma!A2:A30)))</f>
@@ -2994,7 +3016,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E14:S14, Cronograma!A2:A30)))</f>
@@ -3071,7 +3093,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E15:S15, Cronograma!A2:A30)))</f>
@@ -3148,7 +3170,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E16:S16, Cronograma!A2:A30)))</f>
@@ -3225,7 +3247,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E17:S17, Cronograma!A2:A30)))</f>
@@ -3379,7 +3401,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E19:S19, Cronograma!A2:A30)))</f>
@@ -3456,7 +3478,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E20:S20, Cronograma!A2:A30)))</f>
@@ -3610,7 +3632,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E22:S22, Cronograma!A2:A30)))</f>
@@ -3687,7 +3709,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E23:S23, Cronograma!A2:A30)))</f>
@@ -3764,7 +3786,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E24:S24, Cronograma!A2:A30)))</f>
@@ -3841,7 +3863,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E25:S25, Cronograma!A2:A30)))</f>
@@ -3918,7 +3940,7 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E26:S26, Cronograma!A2:A30)))</f>
@@ -4149,7 +4171,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E29:S29, Cronograma!A2:A30)))</f>
@@ -4226,7 +4248,7 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B30">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E30:S30, Cronograma!A2:A30)))</f>
@@ -4380,7 +4402,7 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E32:S32, Cronograma!A2:A30)))</f>
@@ -4457,7 +4479,7 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B33">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E33:S33, Cronograma!A2:A30)))</f>
@@ -4534,7 +4556,7 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E34:S34, Cronograma!A2:A30)))</f>
@@ -4611,7 +4633,7 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E35:S35, Cronograma!A2:A30)))</f>

</xml_diff>

<commit_message>
colores y fromato de fechas
</commit_message>
<xml_diff>
--- a/Cronograma-2026-01-01-2026-01-15.xlsx
+++ b/Cronograma-2026-01-01-2026-01-15.xlsx
@@ -37,12 +37,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="86">
   <si>
     <t>Puestos</t>
   </si>
   <si>
     <t>Nocturno</t>
+  </si>
+  <si>
+    <t>01-01-2026</t>
+  </si>
+  <si>
+    <t>02-01-2026</t>
+  </si>
+  <si>
+    <t>03-01-2026</t>
+  </si>
+  <si>
+    <t>04-01-2026</t>
+  </si>
+  <si>
+    <t>05-01-2026</t>
+  </si>
+  <si>
+    <t>06-01-2026</t>
+  </si>
+  <si>
+    <t>07-01-2026</t>
+  </si>
+  <si>
+    <t>08-01-2026</t>
+  </si>
+  <si>
+    <t>09-01-2026</t>
+  </si>
+  <si>
+    <t>10-01-2026</t>
+  </si>
+  <si>
+    <t>11-01-2026</t>
+  </si>
+  <si>
+    <t>12-01-2026</t>
+  </si>
+  <si>
+    <t>13-01-2026</t>
+  </si>
+  <si>
+    <t>14-01-2026</t>
+  </si>
+  <si>
+    <t>15-01-2026</t>
   </si>
   <si>
     <t>D - L1</t>
@@ -256,9 +301,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -311,12 +353,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -334,21 +373,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF66"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0033CC"/>
+          <bgColor rgb="FF83CCEB"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0DBF33"/>
+          <bgColor rgb="FFB5E6A2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -665,1542 +704,1542 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
-        <v>46023</v>
-      </c>
-      <c r="D1" s="2">
-        <v>46024</v>
-      </c>
-      <c r="E1" s="2">
-        <v>46025</v>
-      </c>
-      <c r="F1" s="2">
-        <v>46026</v>
-      </c>
-      <c r="G1" s="2">
-        <v>46027</v>
-      </c>
-      <c r="H1" s="2">
-        <v>46028</v>
-      </c>
-      <c r="I1" s="2">
-        <v>46029</v>
-      </c>
-      <c r="J1" s="2">
-        <v>46030</v>
-      </c>
-      <c r="K1" s="2">
-        <v>46031</v>
-      </c>
-      <c r="L1" s="2">
-        <v>46032</v>
-      </c>
-      <c r="M1" s="2">
-        <v>46033</v>
-      </c>
-      <c r="N1" s="2">
-        <v>46034</v>
-      </c>
-      <c r="O1" s="2">
-        <v>46035</v>
-      </c>
-      <c r="P1" s="2">
-        <v>46036</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>46037</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="N4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="M5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="Q5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="M6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="Q6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="O7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="Q7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="O8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="M9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="O9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="Q9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="M10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="N10" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="O10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="Q10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="L11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="M11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="O11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="P11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="Q11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="N12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="O12" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="P12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="Q12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="O13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="Q13" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="O14" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="P14" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="Q14" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="M15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="N15" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="O15" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="P15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="Q15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="N16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="O16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="P16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="Q16" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="N17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="O17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="Q17" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J18" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="M18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="O18" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="P18" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="Q18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="I19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="K19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="L19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="M19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="O19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="P19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="Q19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="K20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="L20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="M20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="O20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="P20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="Q20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="K21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="M21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="N21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="O21" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="P21" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="Q21" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" t="s">
         <v>65</v>
       </c>
-      <c r="G22" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" t="s">
-        <v>50</v>
-      </c>
       <c r="J22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="K22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="L22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="M22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="N22" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="O22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="P22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="Q22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" t="s">
         <v>52</v>
       </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" t="s">
-        <v>56</v>
-      </c>
-      <c r="K23" t="s">
-        <v>56</v>
-      </c>
-      <c r="L23" t="s">
-        <v>56</v>
-      </c>
-      <c r="M23" t="s">
-        <v>37</v>
-      </c>
       <c r="P23" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="Q23" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="M24" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="N24" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="P24" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="Q24" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="L25" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="M25" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="N25" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="O25" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="P25" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="Q25" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" t="s">
-        <v>50</v>
-      </c>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="J26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="K26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="L26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="M26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="N26" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="O26" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="P26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="Q26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" t="s">
         <v>66</v>
       </c>
-      <c r="E27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" t="s">
-        <v>51</v>
-      </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="I27" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="L27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="M27" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="N27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="O27" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="P27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="Q27" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="J28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="K28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="L28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="M28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="O28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="P28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="Q28" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="K29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="L29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="M29" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="N29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="O29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="P29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="Q29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="J30" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K30" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="L30" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="M30" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="N30" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="O30" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="P30" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="Q30" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2225,71 +2264,71 @@
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="2">
-        <v>46023</v>
-      </c>
-      <c r="F1" s="2">
-        <v>46024</v>
-      </c>
-      <c r="G1" s="2">
-        <v>46025</v>
-      </c>
-      <c r="H1" s="2">
-        <v>46026</v>
-      </c>
-      <c r="I1" s="2">
-        <v>46027</v>
-      </c>
-      <c r="J1" s="2">
-        <v>46028</v>
-      </c>
-      <c r="K1" s="2">
-        <v>46029</v>
-      </c>
-      <c r="L1" s="2">
-        <v>46030</v>
-      </c>
-      <c r="M1" s="2">
-        <v>46031</v>
-      </c>
-      <c r="N1" s="2">
-        <v>46032</v>
-      </c>
-      <c r="O1" s="2">
-        <v>46033</v>
-      </c>
-      <c r="P1" s="2">
-        <v>46034</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>46035</v>
-      </c>
-      <c r="R1" s="2">
-        <v>46036</v>
-      </c>
-      <c r="S1" s="2">
-        <v>46037</v>
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E2:S2, Cronograma!A2:A30)))</f>
@@ -2366,7 +2405,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E3:S3, Cronograma!A2:A30)))</f>
@@ -2443,7 +2482,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E4:S4, Cronograma!A2:A30)))</f>
@@ -2520,7 +2559,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E5:S5, Cronograma!A2:A30)))</f>
@@ -2597,7 +2636,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E6:S6, Cronograma!A2:A30)))</f>
@@ -2674,7 +2713,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E7:S7, Cronograma!A2:A30)))</f>
@@ -2751,7 +2790,7 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E8:S8, Cronograma!A2:A30)))</f>
@@ -2828,7 +2867,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E9:S9, Cronograma!A2:A30)))</f>
@@ -2905,7 +2944,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E10:S10, Cronograma!A2:A30)))</f>
@@ -2982,7 +3021,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E11:S11, Cronograma!A2:A30)))</f>
@@ -3059,7 +3098,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E12:S12, Cronograma!A2:A30)))</f>
@@ -3136,7 +3175,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B13">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E13:S13, Cronograma!A2:A30)))</f>
@@ -3213,7 +3252,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B14">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E14:S14, Cronograma!A2:A30)))</f>
@@ -3290,7 +3329,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B15">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E15:S15, Cronograma!A2:A30)))</f>
@@ -3367,7 +3406,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E16:S16, Cronograma!A2:A30)))</f>
@@ -3444,7 +3483,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E17:S17, Cronograma!A2:A30)))</f>
@@ -3521,7 +3560,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E18:S18, Cronograma!A2:A30)))</f>
@@ -3598,7 +3637,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E19:S19, Cronograma!A2:A30)))</f>
@@ -3675,7 +3714,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E20:S20, Cronograma!A2:A30)))</f>
@@ -3752,7 +3791,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B21">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E21:S21, Cronograma!A2:A30)))</f>
@@ -3829,7 +3868,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B22">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E22:S22, Cronograma!A2:A30)))</f>
@@ -3906,7 +3945,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B23">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E23:S23, Cronograma!A2:A30)))</f>
@@ -3983,7 +4022,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E24:S24, Cronograma!A2:A30)))</f>
@@ -4060,7 +4099,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B25">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E25:S25, Cronograma!A2:A30)))</f>
@@ -4137,7 +4176,7 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B26">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E26:S26, Cronograma!A2:A30)))</f>
@@ -4214,7 +4253,7 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B27">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E27:S27, Cronograma!A2:A30)))</f>
@@ -4291,7 +4330,7 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E28:S28, Cronograma!A2:A30)))</f>
@@ -4368,7 +4407,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B29">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E29:S29, Cronograma!A2:A30)))</f>
@@ -4445,7 +4484,7 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B30">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E30:S30, Cronograma!A2:A30)))</f>
@@ -4522,7 +4561,7 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B31">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E31:S31, Cronograma!A2:A30)))</f>
@@ -4599,7 +4638,7 @@
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B32">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E32:S32, Cronograma!A2:A30)))</f>
@@ -4676,7 +4715,7 @@
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B33">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E33:S33, Cronograma!A2:A30)))</f>
@@ -4753,7 +4792,7 @@
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B34">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E34:S34, Cronograma!A2:A30)))</f>
@@ -4830,7 +4869,7 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E35:S35, Cronograma!A2:A30)))</f>
@@ -4907,7 +4946,7 @@
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B36">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E36:S36, Cronograma!A2:A30)))</f>
@@ -4984,7 +5023,7 @@
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B37">
         <f>SUMPRODUCT((Cronograma!B2:B30=FALSE) * (COUNTIF(E37:S37, Cronograma!A2:A30)))</f>

</xml_diff>